<commit_message>
Refact the project struct.
</commit_message>
<xml_diff>
--- a/Doc/DBDesign.xlsx
+++ b/Doc/DBDesign.xlsx
@@ -159,9 +159,6 @@
     <t>AliasTable</t>
   </si>
   <si>
-    <t>aliases_name</t>
-  </si>
-  <si>
     <t>standard_name</t>
   </si>
   <si>
@@ -243,6 +240,10 @@
   </si>
   <si>
     <t>Defination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alias_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -578,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -613,7 +614,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
@@ -745,7 +746,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
@@ -763,56 +764,56 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -837,13 +838,13 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -851,13 +852,13 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -865,7 +866,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>23</v>
@@ -877,7 +878,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
@@ -895,42 +896,42 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>